<commit_message>
Updated Origin files for the quantitative data
</commit_message>
<xml_diff>
--- a/endpoints/kettle/admin/quantitative_data/resources/origin/MM260.xlsx
+++ b/endpoints/kettle/admin/quantitative_data/resources/origin/MM260.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="49">
   <si>
     <t>Sector of activity in 3 groups</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>EU27</t>
+  </si>
+  <si>
+    <t>MM260</t>
   </si>
 </sst>
 </file>
@@ -175,7 +178,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -506,31 +509,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -544,6 +547,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -559,15 +571,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -852,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,18 +864,18 @@
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="27"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
@@ -910,8 +913,11 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="20" t="s">
         <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
@@ -942,8 +948,11 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="21" t="s">
         <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
@@ -974,8 +983,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="21" t="s">
         <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>12</v>
@@ -1006,8 +1018,11 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="21" t="s">
         <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>10</v>
@@ -1038,8 +1053,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="21" t="s">
         <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>11</v>
@@ -1070,8 +1088,11 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="21" t="s">
         <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>12</v>
@@ -1102,8 +1123,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="21" t="s">
         <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>10</v>
@@ -1134,8 +1158,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="21" t="s">
         <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>11</v>
@@ -1166,8 +1193,11 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="21" t="s">
         <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>12</v>
@@ -1198,8 +1228,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="21" t="s">
         <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>10</v>
@@ -1230,8 +1263,11 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="21" t="s">
         <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>11</v>
@@ -1262,8 +1298,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="21" t="s">
         <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>12</v>
@@ -1294,8 +1333,11 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="21" t="s">
         <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>10</v>
@@ -1326,8 +1368,11 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="21" t="s">
         <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>11</v>
@@ -1358,8 +1403,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="21" t="s">
         <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>12</v>
@@ -1390,8 +1438,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="21" t="s">
         <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
@@ -1422,8 +1473,11 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="21" t="s">
         <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>11</v>
@@ -1454,8 +1508,11 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="21" t="s">
         <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>12</v>
@@ -1486,8 +1543,11 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="21" t="s">
         <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>10</v>
@@ -1518,8 +1578,11 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="21" t="s">
         <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>11</v>
@@ -1550,8 +1613,11 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="21" t="s">
         <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>12</v>
@@ -1582,8 +1648,11 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="21" t="s">
         <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>10</v>
@@ -1614,8 +1683,11 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="21" t="s">
         <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>11</v>
@@ -1646,8 +1718,11 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="21" t="s">
         <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>12</v>
@@ -1678,8 +1753,11 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="21" t="s">
         <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>10</v>
@@ -1710,8 +1788,11 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="21" t="s">
         <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>11</v>
@@ -1742,8 +1823,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="21" t="s">
         <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>12</v>
@@ -1774,8 +1858,11 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="21" t="s">
         <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>48</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>10</v>
@@ -1806,8 +1893,11 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="21" t="s">
         <v>25</v>
+      </c>
+      <c r="B31" t="s">
+        <v>48</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>11</v>
@@ -1838,8 +1928,11 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="21" t="s">
         <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>12</v>
@@ -1870,8 +1963,11 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="21" t="s">
         <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>48</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>10</v>
@@ -1902,8 +1998,11 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="21" t="s">
         <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>11</v>
@@ -1934,8 +2033,11 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="21" t="s">
         <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>12</v>
@@ -1966,8 +2068,11 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="21" t="s">
         <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>48</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>10</v>
@@ -1998,8 +2103,11 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="21" t="s">
         <v>27</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>11</v>
@@ -2030,8 +2138,11 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="21" t="s">
         <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>12</v>
@@ -2062,8 +2173,11 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="21" t="s">
         <v>28</v>
+      </c>
+      <c r="B39" t="s">
+        <v>48</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>10</v>
@@ -2094,8 +2208,11 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="21" t="s">
         <v>28</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>11</v>
@@ -2126,8 +2243,11 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="21" t="s">
         <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>12</v>
@@ -2158,8 +2278,11 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="26" t="s">
+      <c r="A42" s="21" t="s">
         <v>29</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>10</v>
@@ -2190,8 +2313,11 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="21" t="s">
         <v>29</v>
+      </c>
+      <c r="B43" t="s">
+        <v>48</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>11</v>
@@ -2222,8 +2348,11 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="21" t="s">
         <v>29</v>
+      </c>
+      <c r="B44" t="s">
+        <v>48</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>12</v>
@@ -2254,8 +2383,11 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="21" t="s">
         <v>30</v>
+      </c>
+      <c r="B45" t="s">
+        <v>48</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>10</v>
@@ -2286,8 +2418,11 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="21" t="s">
         <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>48</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>11</v>
@@ -2318,8 +2453,11 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="21" t="s">
         <v>30</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>12</v>
@@ -2350,8 +2488,11 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="21" t="s">
         <v>31</v>
+      </c>
+      <c r="B48" t="s">
+        <v>48</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>10</v>
@@ -2382,8 +2523,11 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="21" t="s">
         <v>31</v>
+      </c>
+      <c r="B49" t="s">
+        <v>48</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>11</v>
@@ -2414,8 +2558,11 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A50" s="26" t="s">
+      <c r="A50" s="21" t="s">
         <v>31</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>12</v>
@@ -2446,8 +2593,11 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="21" t="s">
         <v>32</v>
+      </c>
+      <c r="B51" t="s">
+        <v>48</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>10</v>
@@ -2478,8 +2628,11 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="26" t="s">
+      <c r="A52" s="21" t="s">
         <v>32</v>
+      </c>
+      <c r="B52" t="s">
+        <v>48</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>11</v>
@@ -2510,8 +2663,11 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A53" s="26" t="s">
+      <c r="A53" s="21" t="s">
         <v>32</v>
+      </c>
+      <c r="B53" t="s">
+        <v>48</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>12</v>
@@ -2542,8 +2698,11 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="s">
+      <c r="A54" s="21" t="s">
         <v>33</v>
+      </c>
+      <c r="B54" t="s">
+        <v>48</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>10</v>
@@ -2574,8 +2733,11 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="26" t="s">
+      <c r="A55" s="21" t="s">
         <v>33</v>
+      </c>
+      <c r="B55" t="s">
+        <v>48</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>11</v>
@@ -2606,8 +2768,11 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A56" s="26" t="s">
+      <c r="A56" s="21" t="s">
         <v>33</v>
+      </c>
+      <c r="B56" t="s">
+        <v>48</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>12</v>
@@ -2638,8 +2803,11 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="26" t="s">
+      <c r="A57" s="21" t="s">
         <v>34</v>
+      </c>
+      <c r="B57" t="s">
+        <v>48</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>10</v>
@@ -2670,8 +2838,11 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="26" t="s">
+      <c r="A58" s="21" t="s">
         <v>34</v>
+      </c>
+      <c r="B58" t="s">
+        <v>48</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>11</v>
@@ -2702,8 +2873,11 @@
       </c>
     </row>
     <row r="59" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A59" s="26" t="s">
+      <c r="A59" s="21" t="s">
         <v>34</v>
+      </c>
+      <c r="B59" t="s">
+        <v>48</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>12</v>
@@ -2734,8 +2908,11 @@
       </c>
     </row>
     <row r="60" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="26" t="s">
+      <c r="A60" s="21" t="s">
         <v>35</v>
+      </c>
+      <c r="B60" t="s">
+        <v>48</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>10</v>
@@ -2766,8 +2943,11 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="21" t="s">
         <v>35</v>
+      </c>
+      <c r="B61" t="s">
+        <v>48</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>11</v>
@@ -2798,8 +2978,11 @@
       </c>
     </row>
     <row r="62" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A62" s="26" t="s">
+      <c r="A62" s="21" t="s">
         <v>35</v>
+      </c>
+      <c r="B62" t="s">
+        <v>48</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>12</v>
@@ -2830,8 +3013,11 @@
       </c>
     </row>
     <row r="63" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="26" t="s">
+      <c r="A63" s="21" t="s">
         <v>36</v>
+      </c>
+      <c r="B63" t="s">
+        <v>48</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>10</v>
@@ -2862,8 +3048,11 @@
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="26" t="s">
+      <c r="A64" s="21" t="s">
         <v>36</v>
+      </c>
+      <c r="B64" t="s">
+        <v>48</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>11</v>
@@ -2894,8 +3083,11 @@
       </c>
     </row>
     <row r="65" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A65" s="26" t="s">
+      <c r="A65" s="21" t="s">
         <v>36</v>
+      </c>
+      <c r="B65" t="s">
+        <v>48</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>12</v>
@@ -2926,8 +3118,11 @@
       </c>
     </row>
     <row r="66" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="26" t="s">
+      <c r="A66" s="21" t="s">
         <v>37</v>
+      </c>
+      <c r="B66" t="s">
+        <v>48</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>10</v>
@@ -2958,8 +3153,11 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="26" t="s">
+      <c r="A67" s="21" t="s">
         <v>37</v>
+      </c>
+      <c r="B67" t="s">
+        <v>48</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>11</v>
@@ -2990,8 +3188,11 @@
       </c>
     </row>
     <row r="68" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A68" s="26" t="s">
+      <c r="A68" s="21" t="s">
         <v>37</v>
+      </c>
+      <c r="B68" t="s">
+        <v>48</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>12</v>
@@ -3022,8 +3223,11 @@
       </c>
     </row>
     <row r="69" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="26" t="s">
+      <c r="A69" s="21" t="s">
         <v>38</v>
+      </c>
+      <c r="B69" t="s">
+        <v>48</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>10</v>
@@ -3054,8 +3258,11 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="26" t="s">
+      <c r="A70" s="21" t="s">
         <v>38</v>
+      </c>
+      <c r="B70" t="s">
+        <v>48</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>11</v>
@@ -3086,8 +3293,11 @@
       </c>
     </row>
     <row r="71" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A71" s="26" t="s">
+      <c r="A71" s="21" t="s">
         <v>38</v>
+      </c>
+      <c r="B71" t="s">
+        <v>48</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>12</v>
@@ -3118,8 +3328,11 @@
       </c>
     </row>
     <row r="72" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="26" t="s">
+      <c r="A72" s="21" t="s">
         <v>39</v>
+      </c>
+      <c r="B72" t="s">
+        <v>48</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>10</v>
@@ -3150,8 +3363,11 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="26" t="s">
+      <c r="A73" s="21" t="s">
         <v>39</v>
+      </c>
+      <c r="B73" t="s">
+        <v>48</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>11</v>
@@ -3182,8 +3398,11 @@
       </c>
     </row>
     <row r="74" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A74" s="26" t="s">
+      <c r="A74" s="21" t="s">
         <v>39</v>
+      </c>
+      <c r="B74" t="s">
+        <v>48</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>12</v>
@@ -3214,8 +3433,11 @@
       </c>
     </row>
     <row r="75" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="26" t="s">
+      <c r="A75" s="21" t="s">
         <v>40</v>
+      </c>
+      <c r="B75" t="s">
+        <v>48</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>10</v>
@@ -3246,8 +3468,11 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="26" t="s">
+      <c r="A76" s="21" t="s">
         <v>40</v>
+      </c>
+      <c r="B76" t="s">
+        <v>48</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>11</v>
@@ -3278,8 +3503,11 @@
       </c>
     </row>
     <row r="77" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A77" s="26" t="s">
+      <c r="A77" s="21" t="s">
         <v>40</v>
+      </c>
+      <c r="B77" t="s">
+        <v>48</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>12</v>
@@ -3310,8 +3538,11 @@
       </c>
     </row>
     <row r="78" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="26" t="s">
+      <c r="A78" s="21" t="s">
         <v>41</v>
+      </c>
+      <c r="B78" t="s">
+        <v>48</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>10</v>
@@ -3342,8 +3573,11 @@
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="26" t="s">
+      <c r="A79" s="21" t="s">
         <v>41</v>
+      </c>
+      <c r="B79" t="s">
+        <v>48</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>11</v>
@@ -3374,8 +3608,11 @@
       </c>
     </row>
     <row r="80" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A80" s="26" t="s">
+      <c r="A80" s="21" t="s">
         <v>41</v>
+      </c>
+      <c r="B80" t="s">
+        <v>48</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>12</v>
@@ -3406,8 +3643,11 @@
       </c>
     </row>
     <row r="81" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="26" t="s">
+      <c r="A81" s="21" t="s">
         <v>42</v>
+      </c>
+      <c r="B81" t="s">
+        <v>48</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>10</v>
@@ -3438,8 +3678,11 @@
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="26" t="s">
+      <c r="A82" s="21" t="s">
         <v>42</v>
+      </c>
+      <c r="B82" t="s">
+        <v>48</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>11</v>
@@ -3470,8 +3713,11 @@
       </c>
     </row>
     <row r="83" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A83" s="26" t="s">
+      <c r="A83" s="21" t="s">
         <v>42</v>
+      </c>
+      <c r="B83" t="s">
+        <v>48</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>12</v>
@@ -3502,8 +3748,11 @@
       </c>
     </row>
     <row r="84" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="26" t="s">
+      <c r="A84" s="21" t="s">
         <v>43</v>
+      </c>
+      <c r="B84" t="s">
+        <v>48</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>10</v>
@@ -3534,8 +3783,11 @@
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="26" t="s">
+      <c r="A85" s="21" t="s">
         <v>43</v>
+      </c>
+      <c r="B85" t="s">
+        <v>48</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>11</v>
@@ -3566,8 +3818,11 @@
       </c>
     </row>
     <row r="86" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A86" s="26" t="s">
+      <c r="A86" s="21" t="s">
         <v>43</v>
+      </c>
+      <c r="B86" t="s">
+        <v>48</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>12</v>
@@ -3598,8 +3853,11 @@
       </c>
     </row>
     <row r="87" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="26" t="s">
+      <c r="A87" s="21" t="s">
         <v>44</v>
+      </c>
+      <c r="B87" t="s">
+        <v>48</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>10</v>
@@ -3630,8 +3888,11 @@
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="26" t="s">
+      <c r="A88" s="21" t="s">
         <v>44</v>
+      </c>
+      <c r="B88" t="s">
+        <v>48</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>11</v>
@@ -3662,8 +3923,11 @@
       </c>
     </row>
     <row r="89" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A89" s="26" t="s">
+      <c r="A89" s="21" t="s">
         <v>44</v>
+      </c>
+      <c r="B89" t="s">
+        <v>48</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>12</v>
@@ -3694,8 +3958,11 @@
       </c>
     </row>
     <row r="90" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="26" t="s">
+      <c r="A90" s="21" t="s">
         <v>45</v>
+      </c>
+      <c r="B90" t="s">
+        <v>48</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>10</v>
@@ -3726,8 +3993,11 @@
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" s="26" t="s">
+      <c r="A91" s="21" t="s">
         <v>45</v>
+      </c>
+      <c r="B91" t="s">
+        <v>48</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>11</v>
@@ -3758,8 +4028,11 @@
       </c>
     </row>
     <row r="92" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A92" s="26" t="s">
+      <c r="A92" s="21" t="s">
         <v>45</v>
+      </c>
+      <c r="B92" t="s">
+        <v>48</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>12</v>
@@ -3790,8 +4063,11 @@
       </c>
     </row>
     <row r="93" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="26" t="s">
+      <c r="A93" s="21" t="s">
         <v>46</v>
+      </c>
+      <c r="B93" t="s">
+        <v>48</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>10</v>
@@ -3822,8 +4098,11 @@
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" s="26" t="s">
+      <c r="A94" s="21" t="s">
         <v>46</v>
+      </c>
+      <c r="B94" t="s">
+        <v>48</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>11</v>
@@ -3854,8 +4133,11 @@
       </c>
     </row>
     <row r="95" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A95" s="26" t="s">
+      <c r="A95" s="21" t="s">
         <v>46</v>
+      </c>
+      <c r="B95" t="s">
+        <v>48</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>12</v>
@@ -3886,8 +4168,11 @@
       </c>
     </row>
     <row r="96" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="26" t="s">
+      <c r="A96" s="21" t="s">
         <v>47</v>
+      </c>
+      <c r="B96" t="s">
+        <v>48</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>10</v>
@@ -3918,8 +4203,11 @@
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A97" s="26" t="s">
+      <c r="A97" s="21" t="s">
         <v>47</v>
+      </c>
+      <c r="B97" t="s">
+        <v>48</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>11</v>
@@ -3950,8 +4238,11 @@
       </c>
     </row>
     <row r="98" spans="1:11" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="27" t="s">
+      <c r="A98" s="22" t="s">
         <v>47</v>
+      </c>
+      <c r="B98" t="s">
+        <v>48</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>12</v>

</xml_diff>